<commit_message>
Code cleanup and a few tweeks
</commit_message>
<xml_diff>
--- a/DataLibrary/Data/InterviewTestData.xlsx
+++ b/DataLibrary/Data/InterviewTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>FirstName</t>
   </si>
@@ -194,30 +194,6 @@
   </si>
   <si>
     <t>pwalker2@test.com</t>
-  </si>
-  <si>
-    <t>Rich</t>
-  </si>
-  <si>
-    <t>Cooke</t>
-  </si>
-  <si>
-    <t>Web Developer</t>
-  </si>
-  <si>
-    <t>07909967687</t>
-  </si>
-  <si>
-    <t>richcooke@hotmail.com</t>
-  </si>
-  <si>
-    <t>Danny</t>
-  </si>
-  <si>
-    <t>Mechanic</t>
-  </si>
-  <si>
-    <t>spannermandan@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -764,8 +740,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E15">
-  <autoFilter ref="A1:E15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E13">
+  <autoFilter ref="A1:E13"/>
   <tableColumns count="5">
     <tableColumn id="1" name="FirstName"/>
     <tableColumn id="2" name="LastName"/>
@@ -1074,7 +1050,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1301,40 +1277,6 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>65</v>
-      </c>
-    </row>
   </sheetData>
   <headerFooter/>
   <tableParts>

</xml_diff>